<commit_message>
Done with Lecture 6 R files and homework; correct syllabus
</commit_message>
<xml_diff>
--- a/admin/roster.xlsx
+++ b/admin/roster.xlsx
@@ -1,22 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26230"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ztian/OneDrive/teaching/201702_econometrics/admin/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="12120" windowHeight="8550" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Study Groups" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="137">
   <si>
     <t>学生课堂考勤表</t>
   </si>
@@ -50,7 +60,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="宋体"/>
+        <rFont val="Calibri"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -67,7 +77,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="宋体"/>
+        <rFont val="Calibri"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -85,7 +95,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="宋体"/>
+        <rFont val="Calibri"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -102,7 +112,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="宋体"/>
+        <rFont val="Calibri"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -496,22 +506,37 @@
     <t>8</t>
     <phoneticPr fontId="23" type="noConversion"/>
   </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="24" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -520,7 +545,7 @@
       <b/>
       <sz val="18"/>
       <color theme="3"/>
-      <name val="宋体"/>
+      <name val="Cambria"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="major"/>
@@ -529,7 +554,7 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -538,7 +563,7 @@
       <b/>
       <sz val="13"/>
       <color theme="3"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -547,7 +572,7 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -555,7 +580,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -563,7 +588,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -571,7 +596,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -579,7 +604,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -588,7 +613,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -597,7 +622,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -605,7 +630,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -614,7 +639,7 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -622,7 +647,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -631,7 +656,7 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -640,7 +665,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -648,7 +673,7 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -660,20 +685,20 @@
     </font>
     <font>
       <sz val="12"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="18"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -684,8 +709,14 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -987,14 +1018,14 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1002,10 +1033,10 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1015,32 +1046,32 @@
         <color rgb="FF000000"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -1049,23 +1080,23 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -1197,7 +1228,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -1229,9 +1260,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1244,50 +1272,62 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="165" fontId="21" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="21" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - 强调文字颜色 1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="标题" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="标题 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="标题 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="标题 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="标题 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="差" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="好" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="汇总" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="计算" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="检查单元格" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="解释性文本" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="警告文本" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="链接单元格" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="强调文字颜色 1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="强调文字颜色 2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="强调文字颜色 3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="强调文字颜色 4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="强调文字颜色 5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="强调文字颜色 6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="适中" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="输出" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="输入" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1300,7 +1340,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1342,7 +1382,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1377,7 +1417,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1592,16 +1632,16 @@
       <selection activeCell="A5" sqref="A1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.625" customWidth="1"/>
-    <col min="2" max="2" width="11.875" customWidth="1"/>
+    <col min="1" max="1" width="4.6640625" customWidth="1"/>
+    <col min="2" max="2" width="11.83203125" customWidth="1"/>
     <col min="3" max="3" width="8" customWidth="1"/>
     <col min="4" max="21" width="5.5" customWidth="1"/>
-    <col min="22" max="22" width="7.875" customWidth="1"/>
+    <col min="22" max="22" width="7.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1627,7 +1667,7 @@
       <c r="U1" s="6"/>
       <c r="V1" s="7"/>
     </row>
-    <row r="2" spans="1:22" ht="18.95" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:22" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
@@ -1653,14 +1693,14 @@
       <c r="U2" s="9"/>
       <c r="V2" s="10"/>
     </row>
-    <row r="3" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="12" t="s">
+    <row r="3" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="11" t="s">
         <v>4</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -1717,14 +1757,14 @@
       <c r="U3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="V3" s="14" t="s">
+      <c r="V3" s="13" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="13"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
+    <row r="4" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="12"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
       <c r="D4" s="1" t="s">
         <v>7</v>
       </c>
@@ -1779,9 +1819,9 @@
       <c r="U4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="V4" s="15"/>
-    </row>
-    <row r="5" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="V4" s="14"/>
+    </row>
+    <row r="5" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>1</v>
       </c>
@@ -1811,7 +1851,7 @@
       <c r="U5" s="4"/>
       <c r="V5" s="4"/>
     </row>
-    <row r="6" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>2</v>
       </c>
@@ -1841,7 +1881,7 @@
       <c r="U6" s="4"/>
       <c r="V6" s="4"/>
     </row>
-    <row r="7" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>3</v>
       </c>
@@ -1871,7 +1911,7 @@
       <c r="U7" s="4"/>
       <c r="V7" s="4"/>
     </row>
-    <row r="8" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>4</v>
       </c>
@@ -1901,7 +1941,7 @@
       <c r="U8" s="4"/>
       <c r="V8" s="4"/>
     </row>
-    <row r="9" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>5</v>
       </c>
@@ -1931,7 +1971,7 @@
       <c r="U9" s="4"/>
       <c r="V9" s="4"/>
     </row>
-    <row r="10" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>6</v>
       </c>
@@ -1961,7 +2001,7 @@
       <c r="U10" s="4"/>
       <c r="V10" s="4"/>
     </row>
-    <row r="11" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>7</v>
       </c>
@@ -1991,7 +2031,7 @@
       <c r="U11" s="4"/>
       <c r="V11" s="4"/>
     </row>
-    <row r="12" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>8</v>
       </c>
@@ -2021,7 +2061,7 @@
       <c r="U12" s="4"/>
       <c r="V12" s="4"/>
     </row>
-    <row r="13" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>9</v>
       </c>
@@ -2051,7 +2091,7 @@
       <c r="U13" s="4"/>
       <c r="V13" s="4"/>
     </row>
-    <row r="14" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>10</v>
       </c>
@@ -2081,7 +2121,7 @@
       <c r="U14" s="4"/>
       <c r="V14" s="4"/>
     </row>
-    <row r="15" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>11</v>
       </c>
@@ -2111,7 +2151,7 @@
       <c r="U15" s="4"/>
       <c r="V15" s="4"/>
     </row>
-    <row r="16" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>12</v>
       </c>
@@ -2141,7 +2181,7 @@
       <c r="U16" s="4"/>
       <c r="V16" s="4"/>
     </row>
-    <row r="17" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>13</v>
       </c>
@@ -2171,7 +2211,7 @@
       <c r="U17" s="4"/>
       <c r="V17" s="4"/>
     </row>
-    <row r="18" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>14</v>
       </c>
@@ -2201,7 +2241,7 @@
       <c r="U18" s="4"/>
       <c r="V18" s="4"/>
     </row>
-    <row r="19" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>15</v>
       </c>
@@ -2231,7 +2271,7 @@
       <c r="U19" s="4"/>
       <c r="V19" s="4"/>
     </row>
-    <row r="20" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>16</v>
       </c>
@@ -2261,7 +2301,7 @@
       <c r="U20" s="4"/>
       <c r="V20" s="4"/>
     </row>
-    <row r="21" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>17</v>
       </c>
@@ -2291,7 +2331,7 @@
       <c r="U21" s="4"/>
       <c r="V21" s="4"/>
     </row>
-    <row r="22" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>18</v>
       </c>
@@ -2321,7 +2361,7 @@
       <c r="U22" s="4"/>
       <c r="V22" s="4"/>
     </row>
-    <row r="23" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>19</v>
       </c>
@@ -2351,7 +2391,7 @@
       <c r="U23" s="4"/>
       <c r="V23" s="4"/>
     </row>
-    <row r="24" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>20</v>
       </c>
@@ -2381,7 +2421,7 @@
       <c r="U24" s="4"/>
       <c r="V24" s="4"/>
     </row>
-    <row r="25" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>21</v>
       </c>
@@ -2411,7 +2451,7 @@
       <c r="U25" s="4"/>
       <c r="V25" s="4"/>
     </row>
-    <row r="26" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>22</v>
       </c>
@@ -2441,7 +2481,7 @@
       <c r="U26" s="4"/>
       <c r="V26" s="4"/>
     </row>
-    <row r="27" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>23</v>
       </c>
@@ -2471,7 +2511,7 @@
       <c r="U27" s="4"/>
       <c r="V27" s="4"/>
     </row>
-    <row r="28" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>24</v>
       </c>
@@ -2501,7 +2541,7 @@
       <c r="U28" s="4"/>
       <c r="V28" s="4"/>
     </row>
-    <row r="29" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>25</v>
       </c>
@@ -2531,7 +2571,7 @@
       <c r="U29" s="4"/>
       <c r="V29" s="4"/>
     </row>
-    <row r="30" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>26</v>
       </c>
@@ -2561,7 +2601,7 @@
       <c r="U30" s="4"/>
       <c r="V30" s="4"/>
     </row>
-    <row r="31" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>27</v>
       </c>
@@ -2591,7 +2631,7 @@
       <c r="U31" s="4"/>
       <c r="V31" s="4"/>
     </row>
-    <row r="32" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
         <v>0</v>
       </c>
@@ -2617,7 +2657,7 @@
       <c r="U32" s="6"/>
       <c r="V32" s="7"/>
     </row>
-    <row r="33" spans="1:22" ht="18.95" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:22" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="8" t="s">
         <v>1</v>
       </c>
@@ -2643,14 +2683,14 @@
       <c r="U33" s="9"/>
       <c r="V33" s="10"/>
     </row>
-    <row r="34" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="12" t="s">
+    <row r="34" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B34" s="12" t="s">
+      <c r="B34" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C34" s="12" t="s">
+      <c r="C34" s="11" t="s">
         <v>4</v>
       </c>
       <c r="D34" s="1" t="s">
@@ -2707,14 +2747,14 @@
       <c r="U34" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="V34" s="14" t="s">
+      <c r="V34" s="13" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="13"/>
-      <c r="B35" s="13"/>
-      <c r="C35" s="13"/>
+    <row r="35" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="12"/>
+      <c r="B35" s="12"/>
+      <c r="C35" s="12"/>
       <c r="D35" s="1" t="s">
         <v>7</v>
       </c>
@@ -2769,9 +2809,9 @@
       <c r="U35" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="V35" s="15"/>
-    </row>
-    <row r="36" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="V35" s="14"/>
+    </row>
+    <row r="36" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>28</v>
       </c>
@@ -2801,7 +2841,7 @@
       <c r="U36" s="4"/>
       <c r="V36" s="4"/>
     </row>
-    <row r="37" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>29</v>
       </c>
@@ -2831,7 +2871,7 @@
       <c r="U37" s="4"/>
       <c r="V37" s="4"/>
     </row>
-    <row r="38" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>30</v>
       </c>
@@ -2861,7 +2901,7 @@
       <c r="U38" s="4"/>
       <c r="V38" s="4"/>
     </row>
-    <row r="39" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>31</v>
       </c>
@@ -2891,7 +2931,7 @@
       <c r="U39" s="4"/>
       <c r="V39" s="4"/>
     </row>
-    <row r="40" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>32</v>
       </c>
@@ -2921,7 +2961,7 @@
       <c r="U40" s="4"/>
       <c r="V40" s="4"/>
     </row>
-    <row r="41" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>33</v>
       </c>
@@ -2951,7 +2991,7 @@
       <c r="U41" s="4"/>
       <c r="V41" s="4"/>
     </row>
-    <row r="42" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>34</v>
       </c>
@@ -2981,7 +3021,7 @@
       <c r="U42" s="4"/>
       <c r="V42" s="4"/>
     </row>
-    <row r="43" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>35</v>
       </c>
@@ -3011,7 +3051,7 @@
       <c r="U43" s="4"/>
       <c r="V43" s="4"/>
     </row>
-    <row r="44" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>36</v>
       </c>
@@ -3041,7 +3081,7 @@
       <c r="U44" s="4"/>
       <c r="V44" s="4"/>
     </row>
-    <row r="45" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>37</v>
       </c>
@@ -3071,7 +3111,7 @@
       <c r="U45" s="4"/>
       <c r="V45" s="4"/>
     </row>
-    <row r="46" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>38</v>
       </c>
@@ -3101,7 +3141,7 @@
       <c r="U46" s="4"/>
       <c r="V46" s="4"/>
     </row>
-    <row r="47" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
         <v>39</v>
       </c>
@@ -3131,7 +3171,7 @@
       <c r="U47" s="4"/>
       <c r="V47" s="4"/>
     </row>
-    <row r="48" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <v>40</v>
       </c>
@@ -3161,7 +3201,7 @@
       <c r="U48" s="4"/>
       <c r="V48" s="4"/>
     </row>
-    <row r="49" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <v>41</v>
       </c>
@@ -3191,7 +3231,7 @@
       <c r="U49" s="4"/>
       <c r="V49" s="4"/>
     </row>
-    <row r="50" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
         <v>42</v>
       </c>
@@ -3221,7 +3261,7 @@
       <c r="U50" s="4"/>
       <c r="V50" s="4"/>
     </row>
-    <row r="51" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
         <v>43</v>
       </c>
@@ -3251,7 +3291,7 @@
       <c r="U51" s="4"/>
       <c r="V51" s="4"/>
     </row>
-    <row r="52" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
         <v>44</v>
       </c>
@@ -3281,7 +3321,7 @@
       <c r="U52" s="4"/>
       <c r="V52" s="4"/>
     </row>
-    <row r="53" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
         <v>45</v>
       </c>
@@ -3311,7 +3351,7 @@
       <c r="U53" s="4"/>
       <c r="V53" s="4"/>
     </row>
-    <row r="54" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
         <v>46</v>
       </c>
@@ -3341,7 +3381,7 @@
       <c r="U54" s="4"/>
       <c r="V54" s="4"/>
     </row>
-    <row r="55" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
         <v>47</v>
       </c>
@@ -3371,7 +3411,7 @@
       <c r="U55" s="4"/>
       <c r="V55" s="4"/>
     </row>
-    <row r="56" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
         <v>48</v>
       </c>
@@ -3401,7 +3441,7 @@
       <c r="U56" s="4"/>
       <c r="V56" s="4"/>
     </row>
-    <row r="57" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
         <v>49</v>
       </c>
@@ -3431,7 +3471,7 @@
       <c r="U57" s="4"/>
       <c r="V57" s="4"/>
     </row>
-    <row r="58" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
         <v>50</v>
       </c>
@@ -3461,7 +3501,7 @@
       <c r="U58" s="4"/>
       <c r="V58" s="4"/>
     </row>
-    <row r="59" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
         <v>51</v>
       </c>
@@ -3491,7 +3531,7 @@
       <c r="U59" s="4"/>
       <c r="V59" s="4"/>
     </row>
-    <row r="60" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
         <v>52</v>
       </c>
@@ -3521,7 +3561,7 @@
       <c r="U60" s="4"/>
       <c r="V60" s="4"/>
     </row>
-    <row r="61" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
         <v>53</v>
       </c>
@@ -3551,7 +3591,7 @@
       <c r="U61" s="4"/>
       <c r="V61" s="4"/>
     </row>
-    <row r="62" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="2">
         <v>54</v>
       </c>
@@ -3581,7 +3621,7 @@
       <c r="U62" s="4"/>
       <c r="V62" s="4"/>
     </row>
-    <row r="63" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="5" t="s">
         <v>0</v>
       </c>
@@ -3607,7 +3647,7 @@
       <c r="U63" s="6"/>
       <c r="V63" s="7"/>
     </row>
-    <row r="64" spans="1:22" ht="18.95" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:22" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="8" t="s">
         <v>1</v>
       </c>
@@ -3633,14 +3673,14 @@
       <c r="U64" s="9"/>
       <c r="V64" s="10"/>
     </row>
-    <row r="65" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A65" s="12" t="s">
+    <row r="65" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B65" s="12" t="s">
+      <c r="B65" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C65" s="12" t="s">
+      <c r="C65" s="11" t="s">
         <v>4</v>
       </c>
       <c r="D65" s="1" t="s">
@@ -3697,14 +3737,14 @@
       <c r="U65" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="V65" s="14" t="s">
+      <c r="V65" s="13" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="66" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A66" s="13"/>
-      <c r="B66" s="13"/>
-      <c r="C66" s="13"/>
+    <row r="66" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="12"/>
+      <c r="B66" s="12"/>
+      <c r="C66" s="12"/>
       <c r="D66" s="1" t="s">
         <v>7</v>
       </c>
@@ -3759,9 +3799,9 @@
       <c r="U66" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="V66" s="15"/>
-    </row>
-    <row r="67" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="V66" s="14"/>
+    </row>
+    <row r="67" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="2">
         <v>55</v>
       </c>
@@ -3791,7 +3831,7 @@
       <c r="U67" s="4"/>
       <c r="V67" s="4"/>
     </row>
-    <row r="68" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="2">
         <v>56</v>
       </c>
@@ -3821,7 +3861,7 @@
       <c r="U68" s="4"/>
       <c r="V68" s="4"/>
     </row>
-    <row r="69" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="2">
         <v>57</v>
       </c>
@@ -3851,7 +3891,7 @@
       <c r="U69" s="4"/>
       <c r="V69" s="4"/>
     </row>
-    <row r="70" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="2">
         <v>58</v>
       </c>
@@ -3883,24 +3923,24 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A1:V1"/>
+    <mergeCell ref="A2:V2"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="V3:V4"/>
+    <mergeCell ref="A32:V32"/>
+    <mergeCell ref="A33:V33"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="V34:V35"/>
     <mergeCell ref="A63:V63"/>
     <mergeCell ref="A64:V64"/>
     <mergeCell ref="A65:A66"/>
     <mergeCell ref="B65:B66"/>
     <mergeCell ref="C65:C66"/>
     <mergeCell ref="V65:V66"/>
-    <mergeCell ref="A32:V32"/>
-    <mergeCell ref="A33:V33"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="V34:V35"/>
-    <mergeCell ref="A1:V1"/>
-    <mergeCell ref="A2:V2"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="V3:V4"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.38" right="0.33" top="0.62" bottom="0.73" header="0.4" footer="0.35"/>
@@ -3917,601 +3957,651 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D66"/>
+  <dimension ref="A1:D59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="D54" sqref="D54"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.625" customWidth="1"/>
-    <col min="2" max="2" width="13.25" customWidth="1"/>
-    <col min="3" max="3" width="10.25" customWidth="1"/>
-    <col min="4" max="4" width="9.125" customWidth="1"/>
+    <col min="1" max="1" width="4.6640625" customWidth="1"/>
+    <col min="2" max="2" width="13.1640625" customWidth="1"/>
+    <col min="3" max="3" width="10.1640625" customWidth="1"/>
+    <col min="4" max="4" width="9.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="18" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-    </row>
-    <row r="3" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>33</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
+        <v>35</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>36</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>39</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>34</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>40</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>43</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <v>45</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C10" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D10" s="16" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A4" s="2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
         <v>2</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B11" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C11" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D11" s="16" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A5" s="2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
         <v>3</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B12" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C12" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D12" s="16" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A6" s="2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="2">
+        <v>14</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="2">
+        <v>28</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="2">
+        <v>53</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="2">
+        <v>54</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="2">
+        <v>55</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="2">
+        <v>57</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="2">
+        <v>7</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="2">
+        <v>31</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D20" s="16" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="2">
         <v>4</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B21" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C21" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D21" s="16" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A7" s="2">
-        <v>5</v>
-      </c>
-      <c r="B7" s="3" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="2">
+        <v>5</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C22" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D22" s="16" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A8" s="2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="2">
         <v>6</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B23" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C23" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D23" s="16" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A9" s="2">
-        <v>7</v>
-      </c>
-      <c r="B9" s="3" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="2">
+        <v>25</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D24" s="16" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="2">
+        <v>32</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D25" s="16" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="2">
+        <v>50</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="D26" s="16" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="2">
+        <v>37</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D27" s="16" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="2">
+        <v>41</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D28" s="16" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="2">
+        <v>42</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D29" s="16" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="2">
+        <v>52</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="D30" s="16" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="2">
+        <v>10</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D31" s="16" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="2">
         <v>20</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="B32" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D32" s="16" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="2">
         <v>21</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A10" s="2">
+      <c r="B33" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D33" s="16" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="2">
+        <v>24</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D34" s="16" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="2">
+        <v>19</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D35" s="16" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="2">
+        <v>49</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="D36" s="16" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="2">
+        <v>56</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D37" s="16" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="2">
+        <v>58</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="D38" s="16" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="2">
         <v>8</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B39" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C39" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="4"/>
-    </row>
-    <row r="11" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A11" s="2">
+      <c r="D39" s="16" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="2">
+        <v>13</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D40" s="16" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="2">
+        <v>15</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D41" s="16" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="2">
+        <v>38</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D42" s="16" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="2">
         <v>9</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B43" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C43" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="4"/>
-    </row>
-    <row r="12" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A12" s="2">
-        <v>10</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" s="4"/>
-    </row>
-    <row r="13" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A13" s="2">
+      <c r="D43" s="16" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="2">
         <v>11</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B44" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C44" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="4"/>
-    </row>
-    <row r="14" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A14" s="2">
+      <c r="D44" s="16" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="2">
         <v>12</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B45" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C45" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="4"/>
-    </row>
-    <row r="15" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A15" s="2">
-        <v>13</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D15" s="4"/>
-    </row>
-    <row r="16" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A16" s="2">
-        <v>14</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A17" s="2">
-        <v>15</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D17" s="4"/>
-    </row>
-    <row r="18" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A18" s="2">
-        <v>16</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D18" s="4"/>
-    </row>
-    <row r="19" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A19" s="2">
-        <v>17</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D19" s="4"/>
-    </row>
-    <row r="20" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A20" s="2">
-        <v>18</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D20" s="4"/>
-    </row>
-    <row r="21" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A21" s="2">
-        <v>19</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D21" s="4"/>
-    </row>
-    <row r="22" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A22" s="2">
-        <v>20</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D22" s="4"/>
-    </row>
-    <row r="23" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A23" s="2">
-        <v>21</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D23" s="4"/>
-    </row>
-    <row r="24" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A24" s="2">
-        <v>22</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D24" s="4"/>
-    </row>
-    <row r="25" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A25" s="2">
-        <v>23</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="D25" s="4"/>
-    </row>
-    <row r="26" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A26" s="2">
-        <v>24</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="D26" s="4"/>
-    </row>
-    <row r="27" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A27" s="2">
-        <v>25</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A28" s="2">
-        <v>26</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D28" s="4"/>
-    </row>
-    <row r="29" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A29" s="2">
-        <v>27</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="D29" s="4"/>
-    </row>
-    <row r="30" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A30" s="2">
-        <v>28</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A31" s="2">
-        <v>29</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D31" s="4"/>
-    </row>
-    <row r="32" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A32" s="2">
-        <v>30</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="D32" s="4"/>
-    </row>
-    <row r="33" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A33" s="2">
-        <v>31</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A34" s="2">
-        <v>32</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A35" s="2">
-        <v>33</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A36" s="2">
-        <v>34</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A37" s="2">
-        <v>35</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A38" s="2">
-        <v>36</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A39" s="2">
-        <v>37</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="D39" s="4" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A40" s="2">
-        <v>38</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="D40" s="4"/>
-    </row>
-    <row r="41" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A41" s="2">
-        <v>39</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="D41" s="4" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A42" s="2">
-        <v>40</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="D42" s="4" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A43" s="2">
-        <v>41</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="D43" s="4" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A44" s="2">
-        <v>42</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="D44" s="4" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A45" s="2">
-        <v>43</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="D45" s="4" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="D45" s="15" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>44</v>
       </c>
@@ -4521,201 +4611,174 @@
       <c r="C46" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="D46" s="4"/>
-    </row>
-    <row r="47" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="D46" s="16">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="D47" s="4" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+        <v>99</v>
+      </c>
+      <c r="D47" s="16">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="D48" s="4"/>
-    </row>
-    <row r="49" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+        <v>101</v>
+      </c>
+      <c r="D48" s="16">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
-        <v>47</v>
+        <v>16</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>100</v>
+        <v>38</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="D49" s="4"/>
-    </row>
-    <row r="50" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+        <v>39</v>
+      </c>
+      <c r="D49" s="16"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
+        <v>17</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D50" s="16"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" s="2">
+        <v>18</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D51" s="16"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" s="2">
+        <v>22</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D52" s="16"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" s="2">
+        <v>23</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D53" s="16"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" s="2">
+        <v>26</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D54" s="16"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" s="2">
+        <v>27</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D55" s="16"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" s="2">
+        <v>29</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D56" s="16"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" s="2">
+        <v>30</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D57" s="16"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" s="2">
         <v>48</v>
       </c>
-      <c r="B50" s="3" t="s">
+      <c r="B58" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="C50" s="4" t="s">
+      <c r="C58" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="D50" s="4"/>
-    </row>
-    <row r="51" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A51" s="2">
-        <v>49</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="D51" s="4"/>
-    </row>
-    <row r="52" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A52" s="2">
-        <v>50</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="D52" s="4" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A53" s="2">
+      <c r="D58" s="16"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" s="2">
         <v>51</v>
       </c>
-      <c r="B53" s="3" t="s">
+      <c r="B59" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="C53" s="4" t="s">
+      <c r="C59" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="D53" s="4"/>
-    </row>
-    <row r="54" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A54" s="2">
-        <v>52</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="C54" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="D54" s="4" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A55" s="2">
-        <v>53</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="C55" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="D55" s="4" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A56" s="2">
-        <v>54</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="C56" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="D56" s="4" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A57" s="2">
-        <v>55</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="C57" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="D57" s="4" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A58" s="2">
-        <v>56</v>
-      </c>
-      <c r="B58" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="C58" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="D58" s="4"/>
-    </row>
-    <row r="59" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A59" s="2">
-        <v>57</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="C59" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="D59" s="4" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A60" s="2">
-        <v>58</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="C60" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="D60" s="4"/>
-    </row>
-    <row r="63" spans="1:4" ht="14.25" x14ac:dyDescent="0.15"/>
-    <row r="64" spans="1:4" ht="14.25" x14ac:dyDescent="0.15"/>
-    <row r="65" ht="14.25" x14ac:dyDescent="0.15"/>
-    <row r="66" ht="14.25" x14ac:dyDescent="0.15"/>
+      <c r="D59" s="16"/>
+    </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-  </mergeCells>
+  <sortState ref="A2:D59">
+    <sortCondition ref="D2:D59"/>
+  </sortState>
   <phoneticPr fontId="23" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -4727,7 +4790,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="23" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Half way in lecture 8
</commit_message>
<xml_diff>
--- a/admin/roster.xlsx
+++ b/admin/roster.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Study Groups" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Empirical Exercise" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="681" uniqueCount="139">
   <si>
     <t>学生课堂考勤表</t>
   </si>
@@ -518,13 +518,19 @@
   <si>
     <t>12</t>
   </si>
+  <si>
+    <t>Empirical Exercises</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="25" x14ac:knownFonts="1">
     <font>
@@ -1228,7 +1234,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -1242,6 +1248,19 @@
     <xf numFmtId="49" fontId="21" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="21" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1272,17 +1291,11 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="21" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="1" fontId="21" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1642,65 +1655,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
-      <c r="S1" s="6"/>
-      <c r="T1" s="6"/>
-      <c r="U1" s="6"/>
-      <c r="V1" s="7"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
+      <c r="V1" s="12"/>
     </row>
     <row r="2" spans="1:22" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
-      <c r="N2" s="9"/>
-      <c r="O2" s="9"/>
-      <c r="P2" s="9"/>
-      <c r="Q2" s="9"/>
-      <c r="R2" s="9"/>
-      <c r="S2" s="9"/>
-      <c r="T2" s="9"/>
-      <c r="U2" s="9"/>
-      <c r="V2" s="10"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+      <c r="O2" s="14"/>
+      <c r="P2" s="14"/>
+      <c r="Q2" s="14"/>
+      <c r="R2" s="14"/>
+      <c r="S2" s="14"/>
+      <c r="T2" s="14"/>
+      <c r="U2" s="14"/>
+      <c r="V2" s="15"/>
     </row>
     <row r="3" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="16" t="s">
         <v>4</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -1757,14 +1770,14 @@
       <c r="U3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="V3" s="13" t="s">
+      <c r="V3" s="18" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="12"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
+      <c r="A4" s="17"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
       <c r="D4" s="1" t="s">
         <v>7</v>
       </c>
@@ -1819,7 +1832,7 @@
       <c r="U4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="V4" s="14"/>
+      <c r="V4" s="19"/>
     </row>
     <row r="5" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
@@ -2632,65 +2645,65 @@
       <c r="V31" s="4"/>
     </row>
     <row r="32" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="5" t="s">
+      <c r="A32" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B32" s="6"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="6"/>
-      <c r="G32" s="6"/>
-      <c r="H32" s="6"/>
-      <c r="I32" s="6"/>
-      <c r="J32" s="6"/>
-      <c r="K32" s="6"/>
-      <c r="L32" s="6"/>
-      <c r="M32" s="6"/>
-      <c r="N32" s="6"/>
-      <c r="O32" s="6"/>
-      <c r="P32" s="6"/>
-      <c r="Q32" s="6"/>
-      <c r="R32" s="6"/>
-      <c r="S32" s="6"/>
-      <c r="T32" s="6"/>
-      <c r="U32" s="6"/>
-      <c r="V32" s="7"/>
+      <c r="B32" s="11"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="11"/>
+      <c r="H32" s="11"/>
+      <c r="I32" s="11"/>
+      <c r="J32" s="11"/>
+      <c r="K32" s="11"/>
+      <c r="L32" s="11"/>
+      <c r="M32" s="11"/>
+      <c r="N32" s="11"/>
+      <c r="O32" s="11"/>
+      <c r="P32" s="11"/>
+      <c r="Q32" s="11"/>
+      <c r="R32" s="11"/>
+      <c r="S32" s="11"/>
+      <c r="T32" s="11"/>
+      <c r="U32" s="11"/>
+      <c r="V32" s="12"/>
     </row>
     <row r="33" spans="1:22" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="8" t="s">
+      <c r="A33" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B33" s="9"/>
-      <c r="C33" s="9"/>
-      <c r="D33" s="9"/>
-      <c r="E33" s="9"/>
-      <c r="F33" s="9"/>
-      <c r="G33" s="9"/>
-      <c r="H33" s="9"/>
-      <c r="I33" s="9"/>
-      <c r="J33" s="9"/>
-      <c r="K33" s="9"/>
-      <c r="L33" s="9"/>
-      <c r="M33" s="9"/>
-      <c r="N33" s="9"/>
-      <c r="O33" s="9"/>
-      <c r="P33" s="9"/>
-      <c r="Q33" s="9"/>
-      <c r="R33" s="9"/>
-      <c r="S33" s="9"/>
-      <c r="T33" s="9"/>
-      <c r="U33" s="9"/>
-      <c r="V33" s="10"/>
+      <c r="B33" s="14"/>
+      <c r="C33" s="14"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="14"/>
+      <c r="F33" s="14"/>
+      <c r="G33" s="14"/>
+      <c r="H33" s="14"/>
+      <c r="I33" s="14"/>
+      <c r="J33" s="14"/>
+      <c r="K33" s="14"/>
+      <c r="L33" s="14"/>
+      <c r="M33" s="14"/>
+      <c r="N33" s="14"/>
+      <c r="O33" s="14"/>
+      <c r="P33" s="14"/>
+      <c r="Q33" s="14"/>
+      <c r="R33" s="14"/>
+      <c r="S33" s="14"/>
+      <c r="T33" s="14"/>
+      <c r="U33" s="14"/>
+      <c r="V33" s="15"/>
     </row>
     <row r="34" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="11" t="s">
+      <c r="A34" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B34" s="11" t="s">
+      <c r="B34" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C34" s="11" t="s">
+      <c r="C34" s="16" t="s">
         <v>4</v>
       </c>
       <c r="D34" s="1" t="s">
@@ -2747,14 +2760,14 @@
       <c r="U34" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="V34" s="13" t="s">
+      <c r="V34" s="18" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="35" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="12"/>
-      <c r="B35" s="12"/>
-      <c r="C35" s="12"/>
+      <c r="A35" s="17"/>
+      <c r="B35" s="17"/>
+      <c r="C35" s="17"/>
       <c r="D35" s="1" t="s">
         <v>7</v>
       </c>
@@ -2809,7 +2822,7 @@
       <c r="U35" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="V35" s="14"/>
+      <c r="V35" s="19"/>
     </row>
     <row r="36" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
@@ -3622,65 +3635,65 @@
       <c r="V62" s="4"/>
     </row>
     <row r="63" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="5" t="s">
+      <c r="A63" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B63" s="6"/>
-      <c r="C63" s="6"/>
-      <c r="D63" s="6"/>
-      <c r="E63" s="6"/>
-      <c r="F63" s="6"/>
-      <c r="G63" s="6"/>
-      <c r="H63" s="6"/>
-      <c r="I63" s="6"/>
-      <c r="J63" s="6"/>
-      <c r="K63" s="6"/>
-      <c r="L63" s="6"/>
-      <c r="M63" s="6"/>
-      <c r="N63" s="6"/>
-      <c r="O63" s="6"/>
-      <c r="P63" s="6"/>
-      <c r="Q63" s="6"/>
-      <c r="R63" s="6"/>
-      <c r="S63" s="6"/>
-      <c r="T63" s="6"/>
-      <c r="U63" s="6"/>
-      <c r="V63" s="7"/>
+      <c r="B63" s="11"/>
+      <c r="C63" s="11"/>
+      <c r="D63" s="11"/>
+      <c r="E63" s="11"/>
+      <c r="F63" s="11"/>
+      <c r="G63" s="11"/>
+      <c r="H63" s="11"/>
+      <c r="I63" s="11"/>
+      <c r="J63" s="11"/>
+      <c r="K63" s="11"/>
+      <c r="L63" s="11"/>
+      <c r="M63" s="11"/>
+      <c r="N63" s="11"/>
+      <c r="O63" s="11"/>
+      <c r="P63" s="11"/>
+      <c r="Q63" s="11"/>
+      <c r="R63" s="11"/>
+      <c r="S63" s="11"/>
+      <c r="T63" s="11"/>
+      <c r="U63" s="11"/>
+      <c r="V63" s="12"/>
     </row>
     <row r="64" spans="1:22" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="8" t="s">
+      <c r="A64" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B64" s="9"/>
-      <c r="C64" s="9"/>
-      <c r="D64" s="9"/>
-      <c r="E64" s="9"/>
-      <c r="F64" s="9"/>
-      <c r="G64" s="9"/>
-      <c r="H64" s="9"/>
-      <c r="I64" s="9"/>
-      <c r="J64" s="9"/>
-      <c r="K64" s="9"/>
-      <c r="L64" s="9"/>
-      <c r="M64" s="9"/>
-      <c r="N64" s="9"/>
-      <c r="O64" s="9"/>
-      <c r="P64" s="9"/>
-      <c r="Q64" s="9"/>
-      <c r="R64" s="9"/>
-      <c r="S64" s="9"/>
-      <c r="T64" s="9"/>
-      <c r="U64" s="9"/>
-      <c r="V64" s="10"/>
+      <c r="B64" s="14"/>
+      <c r="C64" s="14"/>
+      <c r="D64" s="14"/>
+      <c r="E64" s="14"/>
+      <c r="F64" s="14"/>
+      <c r="G64" s="14"/>
+      <c r="H64" s="14"/>
+      <c r="I64" s="14"/>
+      <c r="J64" s="14"/>
+      <c r="K64" s="14"/>
+      <c r="L64" s="14"/>
+      <c r="M64" s="14"/>
+      <c r="N64" s="14"/>
+      <c r="O64" s="14"/>
+      <c r="P64" s="14"/>
+      <c r="Q64" s="14"/>
+      <c r="R64" s="14"/>
+      <c r="S64" s="14"/>
+      <c r="T64" s="14"/>
+      <c r="U64" s="14"/>
+      <c r="V64" s="15"/>
     </row>
     <row r="65" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="11" t="s">
+      <c r="A65" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B65" s="11" t="s">
+      <c r="B65" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C65" s="11" t="s">
+      <c r="C65" s="16" t="s">
         <v>4</v>
       </c>
       <c r="D65" s="1" t="s">
@@ -3737,14 +3750,14 @@
       <c r="U65" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="V65" s="13" t="s">
+      <c r="V65" s="18" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="66" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="12"/>
-      <c r="B66" s="12"/>
-      <c r="C66" s="12"/>
+      <c r="A66" s="17"/>
+      <c r="B66" s="17"/>
+      <c r="C66" s="17"/>
       <c r="D66" s="1" t="s">
         <v>7</v>
       </c>
@@ -3799,7 +3812,7 @@
       <c r="U66" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="V66" s="14"/>
+      <c r="V66" s="19"/>
     </row>
     <row r="67" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="2">
@@ -3957,10 +3970,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D59"/>
+  <dimension ref="A1:J60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C65" sqref="C65"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection sqref="A1:F60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3971,813 +3984,1017 @@
     <col min="4" max="4" width="9.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E1" s="9" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D2" s="8" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="2">
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="G2">
+        <v>3</v>
+      </c>
+      <c r="H2">
+        <v>4</v>
+      </c>
+      <c r="I2">
+        <v>5</v>
+      </c>
+      <c r="J2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
         <v>33</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B3" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C3" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D3" s="6" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="2">
+      <c r="F3" s="9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
         <v>35</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B4" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C4" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D4" s="6" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="2">
+      <c r="F4" s="9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
         <v>36</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B5" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C5" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D5" s="6" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
+      <c r="F5" s="9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
         <v>39</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B6" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C6" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D6" s="6" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="2">
+      <c r="F6" s="9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
         <v>34</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B7" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C7" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="D7" s="6" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="2">
+      <c r="F7" s="9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
         <v>40</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B8" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C8" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D8" s="6" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="2">
+      <c r="F8" s="9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
         <v>43</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B9" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C9" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="D8" s="16" t="s">
+      <c r="D9" s="6" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="2">
+      <c r="F9" s="9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
         <v>45</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B10" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C10" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="D10" s="6" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="2">
+      <c r="F10" s="9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
         <v>1</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B11" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C11" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="D11" s="6" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="2">
+      <c r="F11" s="9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
         <v>2</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C12" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="D12" s="6" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="2">
+      <c r="F12" s="9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="2">
         <v>3</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B13" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C13" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="D13" s="6" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="2">
+      <c r="F13" s="9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="2">
         <v>14</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B14" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C14" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D14" s="6" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="2">
+      <c r="F14" s="9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="2">
         <v>28</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B15" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C15" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D14" s="16" t="s">
+      <c r="D15" s="6" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="2">
+      <c r="F15" s="9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="2">
         <v>53</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B16" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C16" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="D15" s="16" t="s">
+      <c r="D16" s="6" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="2">
+      <c r="F16" s="9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="2">
         <v>54</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B17" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C17" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="D16" s="16" t="s">
+      <c r="D17" s="6" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="2">
+      <c r="F17" s="9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="2">
         <v>55</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B18" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C18" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="D17" s="16" t="s">
+      <c r="D18" s="6" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="2">
+      <c r="F18" s="9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="2">
         <v>57</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B19" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C19" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="D18" s="16" t="s">
+      <c r="D19" s="6" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="2">
+      <c r="F19" s="9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="2">
         <v>7</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B20" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C20" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D19" s="16" t="s">
+      <c r="D20" s="6" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="2">
+      <c r="F20" s="9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="2">
         <v>31</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B21" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C21" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="D20" s="16" t="s">
+      <c r="D21" s="6" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="2">
+      <c r="F21" s="9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="2">
         <v>4</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B22" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C22" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D21" s="16" t="s">
+      <c r="D22" s="6" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="2">
+      <c r="F22" s="9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="2">
         <v>5</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B23" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C23" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D22" s="16" t="s">
+      <c r="D23" s="6" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="2">
+      <c r="F23" s="9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="2">
         <v>6</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B24" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C24" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D23" s="16" t="s">
+      <c r="D24" s="6" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="2">
+      <c r="F24" s="9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="2">
         <v>25</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B25" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C25" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="D24" s="16" t="s">
+      <c r="D25" s="6" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="2">
+      <c r="F25" s="9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="2">
         <v>32</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B26" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C26" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D25" s="16" t="s">
+      <c r="D26" s="6" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="2">
+      <c r="F26" s="9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="2">
         <v>50</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B27" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C27" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="D26" s="16" t="s">
+      <c r="D27" s="6" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="2">
+      <c r="F27" s="9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="2">
         <v>37</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B28" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C28" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="D27" s="16" t="s">
+      <c r="D28" s="6" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="2">
+      <c r="F28" s="9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="2">
         <v>41</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B29" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C29" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="D28" s="16" t="s">
+      <c r="D29" s="6" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="2">
+      <c r="F29" s="9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" s="2">
         <v>42</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B30" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C30" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="D29" s="16" t="s">
+      <c r="D30" s="6" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="2">
+      <c r="F30" s="9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" s="2">
         <v>52</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B31" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="C31" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="D30" s="16" t="s">
+      <c r="D31" s="6" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="2">
+      <c r="F31" s="9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" s="2">
         <v>10</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B32" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="C32" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D31" s="16" t="s">
+      <c r="D32" s="6" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="2">
+      <c r="F32" s="9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" s="2">
         <v>20</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B33" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="C33" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D32" s="16" t="s">
+      <c r="D33" s="6" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="2">
+      <c r="F33" s="9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="2">
         <v>21</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B34" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="C34" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D33" s="16" t="s">
+      <c r="D34" s="6" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="2">
+      <c r="F34" s="9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" s="2">
         <v>24</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B35" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="C35" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D34" s="16" t="s">
+      <c r="D35" s="6" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="2">
+      <c r="F35" s="9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="2">
         <v>19</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B36" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C35" s="4" t="s">
+      <c r="C36" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D35" s="16" t="s">
+      <c r="D36" s="6" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="2">
+      <c r="F36" s="9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="2">
         <v>49</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B37" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="C36" s="4" t="s">
+      <c r="C37" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="D36" s="16" t="s">
+      <c r="D37" s="6" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="2">
+      <c r="F37" s="9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" s="2">
         <v>56</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B38" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="C38" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="D37" s="16" t="s">
+      <c r="D38" s="6" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="2">
+      <c r="F38" s="9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" s="2">
         <v>58</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B39" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="C38" s="4" t="s">
+      <c r="C39" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="D38" s="16" t="s">
+      <c r="D39" s="6" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" s="2">
+      <c r="F39" s="9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" s="2">
         <v>8</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B40" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C39" s="4" t="s">
+      <c r="C40" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D39" s="16" t="s">
+      <c r="D40" s="6" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" s="2">
+      <c r="F40" s="9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" s="2">
         <v>13</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B41" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C40" s="4" t="s">
+      <c r="C41" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D40" s="16" t="s">
+      <c r="D41" s="6" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" s="2">
+      <c r="F41" s="9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" s="2">
         <v>15</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="B42" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C41" s="4" t="s">
+      <c r="C42" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D41" s="16" t="s">
+      <c r="D42" s="6" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" s="2">
+      <c r="F42" s="9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" s="2">
         <v>38</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="B43" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="C42" s="4" t="s">
+      <c r="C43" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="D42" s="16" t="s">
+      <c r="D43" s="6" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="2">
+      <c r="F43" s="9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" s="2">
         <v>9</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B44" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C43" s="4" t="s">
+      <c r="C44" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D43" s="16" t="s">
+      <c r="D44" s="6" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" s="2">
+      <c r="F44" s="9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" s="2">
         <v>11</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="B45" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C44" s="4" t="s">
+      <c r="C45" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D44" s="16" t="s">
+      <c r="D45" s="6" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="2">
+      <c r="F45" s="9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" s="2">
         <v>12</v>
       </c>
-      <c r="B45" s="3" t="s">
+      <c r="B46" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C45" s="4" t="s">
+      <c r="C46" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D45" s="15" t="s">
+      <c r="D46" s="5" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" s="2">
+      <c r="F46" s="9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" s="2">
         <v>44</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="B47" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="C46" s="4" t="s">
+      <c r="C47" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="D46" s="16">
+      <c r="D47" s="6">
         <v>13</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" s="2">
+      <c r="F47" s="9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" s="2">
         <v>46</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="B48" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="C47" s="4" t="s">
+      <c r="C48" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="D47" s="16">
+      <c r="D48" s="6">
         <v>13</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48" s="2">
+      <c r="F48" s="9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" s="2">
         <v>47</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="B49" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="C48" s="4" t="s">
+      <c r="C49" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="D48" s="16">
+      <c r="D49" s="6">
         <v>13</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" s="2">
+      <c r="F49" s="9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50" s="2">
+        <v>22</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D50" s="6">
+        <v>14</v>
+      </c>
+      <c r="F50" s="9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" s="2">
+        <v>27</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D51" s="6">
+        <v>14</v>
+      </c>
+      <c r="F51" s="9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52" s="2">
         <v>16</v>
       </c>
-      <c r="B49" s="3" t="s">
+      <c r="B52" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C49" s="4" t="s">
+      <c r="C52" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D49" s="16"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" s="2">
+      <c r="D52" s="6">
+        <v>15</v>
+      </c>
+      <c r="F52" s="9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53" s="2">
         <v>17</v>
       </c>
-      <c r="B50" s="3" t="s">
+      <c r="B53" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C50" s="4" t="s">
+      <c r="C53" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D50" s="16"/>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" s="2">
+      <c r="D53" s="6">
+        <v>15</v>
+      </c>
+      <c r="F53" s="9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54" s="2">
+        <v>30</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D54" s="6">
+        <v>15</v>
+      </c>
+      <c r="F54" s="9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A55" s="2">
+        <v>48</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D55" s="6">
+        <v>15</v>
+      </c>
+      <c r="F55" s="9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56" s="2">
+        <v>51</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D56" s="6">
+        <v>15</v>
+      </c>
+      <c r="F56" s="9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A57" s="2">
+        <v>23</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D57" s="6">
+        <v>16</v>
+      </c>
+      <c r="F57" s="9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A58" s="2">
         <v>18</v>
       </c>
-      <c r="B51" s="3" t="s">
+      <c r="B58" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C51" s="4" t="s">
+      <c r="C58" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D51" s="16"/>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52" s="2">
-        <v>22</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D52" s="16"/>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" s="2">
-        <v>23</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="D53" s="16"/>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A54" s="2">
+      <c r="D58" s="6"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A59" s="2">
         <v>26</v>
       </c>
-      <c r="B54" s="3" t="s">
+      <c r="B59" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C54" s="4" t="s">
+      <c r="C59" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="D54" s="16"/>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55" s="2">
-        <v>27</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="C55" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="D55" s="16"/>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" s="2">
+      <c r="D59" s="6"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A60" s="2">
         <v>29</v>
       </c>
-      <c r="B56" s="3" t="s">
+      <c r="B60" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C56" s="4" t="s">
+      <c r="C60" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="D56" s="16"/>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57" s="2">
-        <v>30</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="C57" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="D57" s="16"/>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" s="2">
-        <v>48</v>
-      </c>
-      <c r="B58" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="C58" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="D58" s="16"/>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" s="2">
-        <v>51</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="C59" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="D59" s="16"/>
+      <c r="D60" s="6"/>
     </row>
   </sheetData>
-  <sortState ref="A2:D59">
-    <sortCondition ref="D2:D59"/>
+  <sortState ref="A3:J60">
+    <sortCondition ref="D3:D60"/>
   </sortState>
   <phoneticPr fontId="23" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4786,12 +5003,1010 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="164" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="5" max="5" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="20" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="E1">
+        <v>1</v>
+      </c>
+      <c r="F1" s="20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>33</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>35</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="F3" s="21" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>36</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="F4" s="21" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>39</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="F5" s="21" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>34</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="F6" s="21" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>40</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="F7" s="21" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>43</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="F8" s="21" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <v>45</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="F9" s="21" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
+        <v>1</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="F10" s="21" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
+        <v>2</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="F11" s="21" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
+        <v>3</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="F12" s="21" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="2">
+        <v>14</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="F13" s="21" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="2">
+        <v>28</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="F14" s="21" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="2">
+        <v>53</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="F15" s="21" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="2">
+        <v>54</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="F16" s="21" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="2">
+        <v>55</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="F17" s="21" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="2">
+        <v>57</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="F18" s="21" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="2">
+        <v>7</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="F19" s="21" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="2">
+        <v>31</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="F20" s="21" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="2">
+        <v>4</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="F21" s="21" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="2">
+        <v>5</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="F22" s="21" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="2">
+        <v>6</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="F23" s="21" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="2">
+        <v>25</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="F24" s="21" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="2">
+        <v>32</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="F25" s="21" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="2">
+        <v>50</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="F26" s="21" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="2">
+        <v>37</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="F27" s="21" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="2">
+        <v>41</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="F28" s="21" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="2">
+        <v>42</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="F29" s="21" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" s="2">
+        <v>52</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="F30" s="21" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" s="2">
+        <v>10</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="F31" s="21" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" s="2">
+        <v>20</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="F32" s="21" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" s="2">
+        <v>21</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="F33" s="21" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="2">
+        <v>24</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="F34" s="21" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" s="2">
+        <v>19</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="F35" s="21" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="2">
+        <v>49</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="F36" s="21" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="2">
+        <v>56</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="F37" s="21" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" s="2">
+        <v>58</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="F38" s="21" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" s="2">
+        <v>8</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="F39" s="21" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" s="2">
+        <v>13</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="F40" s="21" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" s="2">
+        <v>15</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="F41" s="21" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" s="2">
+        <v>38</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="F42" s="21" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" s="2">
+        <v>9</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="F43" s="21" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" s="2">
+        <v>11</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="F44" s="21" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" s="2">
+        <v>12</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="F45" s="21" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" s="2">
+        <v>44</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D46" s="6">
+        <v>13</v>
+      </c>
+      <c r="F46" s="21" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" s="2">
+        <v>46</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="D47" s="6">
+        <v>13</v>
+      </c>
+      <c r="F47" s="21" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" s="2">
+        <v>47</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D48" s="6">
+        <v>13</v>
+      </c>
+      <c r="F48" s="21" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" s="2">
+        <v>22</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D49" s="6">
+        <v>14</v>
+      </c>
+      <c r="F49" s="21" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50" s="2">
+        <v>27</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D50" s="6">
+        <v>14</v>
+      </c>
+      <c r="F50" s="21" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" s="2">
+        <v>16</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D51" s="6">
+        <v>15</v>
+      </c>
+      <c r="F51" s="21" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52" s="2">
+        <v>17</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D52" s="6">
+        <v>15</v>
+      </c>
+      <c r="F52" s="21" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53" s="2">
+        <v>30</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D53" s="6">
+        <v>15</v>
+      </c>
+      <c r="F53" s="21" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54" s="2">
+        <v>48</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D54" s="6">
+        <v>15</v>
+      </c>
+      <c r="F54" s="21" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A55" s="2">
+        <v>51</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D55" s="6">
+        <v>15</v>
+      </c>
+      <c r="F55" s="21" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56" s="2">
+        <v>23</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D56" s="6">
+        <v>16</v>
+      </c>
+      <c r="F56" s="21" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A57" s="2">
+        <v>18</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D57" s="6"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A58" s="2">
+        <v>26</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D58" s="6"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A59" s="2">
+        <v>29</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D59" s="6"/>
+    </row>
+  </sheetData>
   <phoneticPr fontId="23" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>